<commit_message>
Set up search male thread.
</commit_message>
<xml_diff>
--- a/docs/questions.xlsx
+++ b/docs/questions.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\workspace\Colloquy\exposition\docs\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{8402CE63-9938-4FEC-95E4-55122389EC69}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D7371EF2-0D84-4304-91FB-A45C61644CDC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="24220" windowHeight="15500" xr2:uid="{09E106AB-5E23-40BC-B463-646C6FB80B32}"/>
+    <workbookView xWindow="3420" yWindow="3420" windowWidth="18000" windowHeight="11170" xr2:uid="{09E106AB-5E23-40BC-B463-646C6FB80B32}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -34,9 +34,27 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1" uniqueCount="1">
-  <si>
-    <t>The male/neopixel/ring always white.</t>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="7" uniqueCount="7">
+  <si>
+    <t>O drive max = 255 (max pixel brightness) ?</t>
+  </si>
+  <si>
+    <t>The male/neopixel/ring always white ?</t>
+  </si>
+  <si>
+    <t>O drive max = 0 (pixel shutdown) ?</t>
+  </si>
+  <si>
+    <t>P drive max = 255 (max pixel brightness) ?</t>
+  </si>
+  <si>
+    <t>P drive max = 0 (pixel shutdown) ?</t>
+  </si>
+  <si>
+    <t>P drive increment X unit every Y seconds. X and Y ?</t>
+  </si>
+  <si>
+    <t>O drive increment X unit every Y seconds. X and Y ?</t>
   </si>
 </sst>
 </file>
@@ -388,20 +406,50 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{01568BC7-098F-4810-AAF9-0B457EB4AF2B}">
-  <dimension ref="A1"/>
+  <dimension ref="A2:A8"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="I11" sqref="I11"/>
+      <selection activeCell="A9" sqref="A9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="32.54296875" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="48.54296875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:1" x14ac:dyDescent="0.35">
-      <c r="A1" t="s">
+    <row r="2" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A2" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="3" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A3" t="s">
         <v>0</v>
+      </c>
+    </row>
+    <row r="4" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A4" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="5" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A5" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="6" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A6" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="7" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A7" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="8" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A8" t="s">
+        <v>6</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Set up test framework.
</commit_message>
<xml_diff>
--- a/docs/questions.xlsx
+++ b/docs/questions.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\workspace\Colloquy\exposition\docs\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{60085848-2321-47E1-A70C-171B95C0A671}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3CAA7F78-966C-4999-9E77-1802EB8ECD50}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="3420" yWindow="3420" windowWidth="18000" windowHeight="11170" xr2:uid="{09E106AB-5E23-40BC-B463-646C6FB80B32}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="24220" windowHeight="15500" xr2:uid="{09E106AB-5E23-40BC-B463-646C6FB80B32}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="10" uniqueCount="10">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="18" uniqueCount="18">
   <si>
     <t>O drive max = 255 (max pixel brightness) ?</t>
   </si>
@@ -133,6 +133,357 @@
   </si>
   <si>
     <t>How many interactions are expecting every hour ?</t>
+  </si>
+  <si>
+    <t>Should the female start to flaps the mirror immediatly after a sensing a male or should it sense the beam first ?</t>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">What is the exact </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>female</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>sound</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> pattern to notify a male that she is interested ?</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">What is the exact </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>light</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> pattern for the </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">male </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>while</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> searching</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> ?</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">What is the exact climax </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>light</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> and </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>sound</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> pattern for the </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>female</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> ?</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">What is the exact climax </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>light</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> and </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>sound</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> pattern for the </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>male</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> ?</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">What is the exact </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>male</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> encouragement </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>sound</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> pattern ?</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">Does the </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>mirror</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> has a search state when the female </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>doesn't remember</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> the male ? (search state would be stop when the encourement signal is heard.)</t>
+    </r>
+  </si>
+  <si>
+    <t>victor</t>
   </si>
 </sst>
 </file>
@@ -492,65 +843,105 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{01568BC7-098F-4810-AAF9-0B457EB4AF2B}">
-  <dimension ref="A2:A11"/>
+  <dimension ref="A1:B18"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A11" sqref="A11"/>
+      <selection activeCell="B11" sqref="B11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="87.08984375" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="128.1796875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="B1" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A2" t="s">
         <v>7</v>
       </c>
     </row>
-    <row r="3" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A3" t="s">
         <v>0</v>
       </c>
     </row>
-    <row r="4" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A4" t="s">
         <v>4</v>
       </c>
     </row>
-    <row r="5" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A5" t="s">
         <v>1</v>
       </c>
     </row>
-    <row r="6" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A6" t="s">
         <v>5</v>
       </c>
     </row>
-    <row r="7" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="7" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A7" t="s">
         <v>2</v>
       </c>
     </row>
-    <row r="8" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="8" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A8" t="s">
         <v>3</v>
       </c>
     </row>
-    <row r="9" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="9" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A9" t="s">
         <v>8</v>
       </c>
     </row>
-    <row r="10" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="10" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A10" t="s">
         <v>6</v>
       </c>
     </row>
-    <row r="11" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="11" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A11" t="s">
         <v>9</v>
+      </c>
+    </row>
+    <row r="12" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A12" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="13" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A13" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="14" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A14" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="15" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A15" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="16" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A16" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="17" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A17" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="18" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A18" t="s">
+        <v>16</v>
       </c>
     </row>
   </sheetData>

</xml_diff>